<commit_message>
Cargos descuentos incluir campo indicador de descuento, tributos incluir los codigos de impuestos cabecera sin repeticiones
Cargos descuentos incluir campo indicador de descuento, tributos incluir los codigos de impuestos cabecera sin repeticiones
</commit_message>
<xml_diff>
--- a/doc/CalidadYPruebas/190822 getty colombia plan de pruebas factura electronica.xlsx
+++ b/doc/CalidadYPruebas/190822 getty colombia plan de pruebas factura electronica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\jcTii\Desarrollo\COL_FacturaElectronica\co02\doc\CalidadYPruebas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositorio local\co02\doc\CalidadYPruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130727ED-738E-4081-A335-001324FF1559}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968E3C08-B813-4909-878A-5E23493EF845}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2895" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="facturaelectronica" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Factura  Electrónica Colombia</t>
   </si>
@@ -183,6 +183,9 @@
     <t xml:space="preserve">Transacciones/Ventas/Entrada de transacción de ventas
 Seleccionar el cliente Lowe
 Emitir factura con la Aplicación de emisión de factura electrónica  </t>
+  </si>
+  <si>
+    <t>&gt;</t>
   </si>
 </sst>
 </file>
@@ -366,7 +369,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -664,11 +667,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
@@ -772,8 +775,8 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>4</v>
+      <c r="A7" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>9</v>

</xml_diff>